<commit_message>
Everything readied for the poster
</commit_message>
<xml_diff>
--- a/MLStats.xlsx
+++ b/MLStats.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Classification Type</t>
   </si>
@@ -77,6 +77,9 @@
     <t>72.498s</t>
   </si>
   <si>
+    <t>SGD</t>
+  </si>
+  <si>
     <t>KNN</t>
   </si>
   <si>
@@ -93,14 +96,49 @@
   </si>
   <si>
     <t>85.838s</t>
+  </si>
+  <si>
+    <t>83.264s</t>
+  </si>
+  <si>
+    <t>More Filtration</t>
+  </si>
+  <si>
+    <t>1.139s</t>
+  </si>
+  <si>
+    <t>1.074s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SVM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>1.119s</t>
+  </si>
+  <si>
+    <t>93.51s</t>
+  </si>
+  <si>
+    <t>24.358s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -128,8 +166,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,13 +532,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>149</v>
@@ -539,13 +578,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>140</v>
@@ -585,13 +624,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8">
         <v>155</v>
@@ -608,10 +647,145 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>159</v>
+      </c>
+      <c r="E9">
+        <v>0.96389999999999998</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>146</v>
+      </c>
+      <c r="E12">
+        <v>0.88480000000000003</v>
+      </c>
+      <c r="F12">
+        <v>19</v>
+      </c>
+      <c r="G12">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <v>127</v>
+      </c>
+      <c r="E13">
+        <v>0.76968999999999999</v>
+      </c>
+      <c r="F13">
+        <v>21</v>
+      </c>
+      <c r="G13">
+        <v>0.65625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>126</v>
+      </c>
+      <c r="E14">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="F14">
+        <v>26</v>
+      </c>
+      <c r="G14">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>165</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16">
+        <v>144</v>
+      </c>
+      <c r="E16">
+        <v>0.87270000000000003</v>
+      </c>
+      <c r="F16">
+        <v>22</v>
+      </c>
+      <c r="G16">
+        <v>0.6875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Almost done, need to add a few more things to the report and fix LSTM
</commit_message>
<xml_diff>
--- a/MLStats.xlsx
+++ b/MLStats.xlsx
@@ -1,36 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brandon/Documents/Stanford 16-17/Classes/Fall Quarter/CS 221/Project/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33520" windowHeight="20540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9880" yWindow="0" windowWidth="25600" windowHeight="14740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Remission Dataset" sheetId="1" r:id="rId1"/>
-    <sheet name="Remission" sheetId="2" r:id="rId2"/>
-    <sheet name="Kidney" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
+    <sheet name="F1 Scores" sheetId="6" r:id="rId2"/>
+    <sheet name="Remission" sheetId="2" r:id="rId3"/>
+    <sheet name="Kidney" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>Classification Type</t>
   </si>
@@ -138,6 +134,27 @@
   </si>
   <si>
     <t>KNN - heavily filtered</t>
+  </si>
+  <si>
+    <t>True Negatives</t>
+  </si>
+  <si>
+    <t>False Negatives</t>
+  </si>
+  <si>
+    <t>False Positives</t>
+  </si>
+  <si>
+    <t>True Positives</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1</t>
   </si>
 </sst>
 </file>
@@ -278,7 +295,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -304,20 +320,91 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Remission!$B$9:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-              </c:numCache>
-            </c:numRef>
+            <c:strRef>
+              <c:f>Remission!$B$9:$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>SVM - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SGD - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LogReg - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>KNN - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SVM - filtered</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SGD -filtered</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>LogReg - filtered</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>KNN - filtered</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SGD - All</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SVM - all</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Logreg - all</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>KNN - all</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Remission!$C$9:$C$16</c:f>
+              <c:f>Remission!$C$9:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.2141</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.054</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.156</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.867</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.992</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.931</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.872</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>79.18000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72.498</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>85.838</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>83.264</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -331,11 +418,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2103708832"/>
-        <c:axId val="2144180320"/>
+        <c:axId val="2111916920"/>
+        <c:axId val="2111919960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2103708832"/>
+        <c:axId val="2111916920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -355,7 +442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144180320"/>
+        <c:crossAx val="2111919960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -363,7 +450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144180320"/>
+        <c:axId val="2111919960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -386,7 +473,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -403,7 +489,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103708832"/>
+        <c:crossAx val="2111916920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -465,7 +551,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -474,26 +559,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -602,11 +667,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2103523280"/>
-        <c:axId val="2125060592"/>
+        <c:axId val="2097908264"/>
+        <c:axId val="2100962872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2103523280"/>
+        <c:axId val="2097908264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -638,7 +703,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -647,26 +711,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -705,7 +749,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125060592"/>
+        <c:crossAx val="2100962872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -713,7 +757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2125060592"/>
+        <c:axId val="2100962872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -759,7 +803,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -768,27 +811,8 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -819,7 +843,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103523280"/>
+        <c:crossAx val="2097908264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -904,31 +928,43 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$10:$B$17</c:f>
+              <c:f>Sheet2!$B$6:$B$17</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>SVM - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SGD - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LogReg - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>KNN - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>SVM - filtered</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>SGD - filtered</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>LogReg - filtered</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>KNN - filtered</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>SVM - all</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>SGD - all</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>Logreg - all</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>KNN - all</c:v>
                 </c:pt>
               </c:strCache>
@@ -936,32 +972,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$C$10:$C$17</c:f>
+              <c:f>Sheet2!$C$6:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.7272</c:v>
+                  <c:v>0.8125</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.59375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.65625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7185</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.78125</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>0.90303</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>0.8484</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>0.8121</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>0.7815</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>0.9393</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>0.9639</c:v>
                 </c:pt>
               </c:numCache>
@@ -985,31 +1033,43 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$10:$B$17</c:f>
+              <c:f>Sheet2!$B$6:$B$17</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>SVM - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SGD - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LogReg - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>KNN - heavily filtered</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>SVM - filtered</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
                   <c:v>SGD - filtered</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>LogReg - filtered</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>KNN - filtered</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>SVM - all</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>SGD - all</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>Logreg - all</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>KNN - all</c:v>
                 </c:pt>
               </c:strCache>
@@ -1017,32 +1077,44 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$10:$D$17</c:f>
+              <c:f>Sheet2!$D$6:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.7185</c:v>
+                  <c:v>0.7636</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.7757</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8848</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76969</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7272</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.58181</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
                   <c:v>0.53125</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="7">
                   <c:v>0.46875</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>0.4375</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
                   <c:v>0.296969</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>0.1875</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>0.0625</c:v>
                 </c:pt>
               </c:numCache>
@@ -1060,11 +1132,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1819012752"/>
-        <c:axId val="2144583344"/>
+        <c:axId val="2097775000"/>
+        <c:axId val="2097155064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1819012752"/>
+        <c:axId val="2097775000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,7 +1156,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144583344"/>
+        <c:crossAx val="2097155064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1092,13 +1164,31 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144583344"/>
+        <c:axId val="2097155064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Classification Accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1113,14 +1203,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1819012752"/>
+        <c:crossAx val="2097775000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1692,10 +1781,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
@@ -1765,13 +1854,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2048,7 +2137,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2059,10 +2148,10 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G8"/>
+      <selection activeCell="F1" sqref="F1:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
@@ -2071,7 +2160,7 @@
     <col min="6" max="7" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2094,7 +2183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2117,7 +2206,7 @@
         <v>0.71850000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2140,7 +2229,7 @@
         <v>0.59375</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2163,7 +2252,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2186,7 +2275,7 @@
         <v>0.46875</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2209,7 +2298,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -2232,7 +2321,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2255,7 +2344,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -2281,23 +2370,414 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:C24"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>126</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>39</v>
+      </c>
+      <c r="F2">
+        <f>D2/(D2+E2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="G2">
+        <f>D2/(D2+C2)</f>
+        <v>0.8125</v>
+      </c>
+      <c r="H2">
+        <f xml:space="preserve"> 2 * (F2*G2)/(F2+G3)</f>
+        <v>0.65408805031446537</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>128</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>37</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F12" si="0">D3/(D3+E3)</f>
+        <v>0.3392857142857143</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G12" si="1">D3/(D3+C3)</f>
+        <v>0.59375</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H12" si="2" xml:space="preserve"> 2 * (F3*G3)/(F3+G4)</f>
+        <v>0.43181818181818188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>146</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>0.59375</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>0.51351351351351349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>127</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>38</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.3559322033898305</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0.65625</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>0.4346968950221784</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>120</v>
+      </c>
+      <c r="C6">
+        <f>32-D6</f>
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <f>165-B6</f>
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.33823529411764708</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.71875</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>0.52169625246548323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>121</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C12" si="3">32-D7</f>
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E12" si="4">165-B7</f>
+        <v>44</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.30158730158730157</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.59375</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>0.43001786777843953</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>149</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.51515151515151514</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.53125</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>0.55630413859480277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>140</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.46875</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0.43269230769230771</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>134</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.4375</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>0.5459610027855154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>155</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.1875</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0.32142857142857145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>159</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B8:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -2305,67 +2785,99 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>1.2141</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>1.054</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>1.1559999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>2.867</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>2.992</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>2.931</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>1.8720000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C17">
-        <v>2.867</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+        <v>79.180000000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
       <c r="B18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C18">
-        <v>2.992</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+        <v>72.498000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
       <c r="B19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C19">
-        <v>2.931</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+        <v>85.837999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
       <c r="B20" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C20">
-        <v>1.8720000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21">
-        <v>79.180000000000007</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22">
-        <v>72.498000000000005</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23">
-        <v>85.837999999999994</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24">
         <v>83.263999999999996</v>
       </c>
     </row>
@@ -2374,10 +2886,15 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C12:D20"/>
   <sheetViews>
@@ -2385,9 +2902,9 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:4">
       <c r="C12" t="s">
         <v>25</v>
       </c>
@@ -2395,7 +2912,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:4">
       <c r="C13" t="s">
         <v>18</v>
       </c>
@@ -2403,7 +2920,7 @@
         <v>1.893</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:4">
       <c r="C14" t="s">
         <v>27</v>
       </c>
@@ -2411,7 +2928,7 @@
         <v>2.1030000000000002</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:4">
       <c r="C15" t="s">
         <v>20</v>
       </c>
@@ -2419,7 +2936,7 @@
         <v>2.4670000000000001</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:4">
       <c r="C16" t="s">
         <v>21</v>
       </c>
@@ -2427,7 +2944,7 @@
         <v>1.915</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:4">
       <c r="C17" t="s">
         <v>28</v>
       </c>
@@ -2435,7 +2952,7 @@
         <v>14.669</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:4">
       <c r="C18" t="s">
         <v>22</v>
       </c>
@@ -2443,7 +2960,7 @@
         <v>13.388999999999999</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:4">
       <c r="C19" t="s">
         <v>23</v>
       </c>
@@ -2451,7 +2968,7 @@
         <v>17.917999999999999</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:4">
       <c r="C20" t="s">
         <v>24</v>
       </c>
@@ -2462,10 +2979,15 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:D17"/>
   <sheetViews>
@@ -2473,13 +2995,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>25</v>
       </c>
@@ -2490,44 +3012,62 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>0.8125</v>
+      </c>
+      <c r="D6">
+        <v>0.76359999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
       <c r="B7" t="s">
         <v>33</v>
       </c>
       <c r="C7">
-        <v>0.8125</v>
+        <v>0.59375</v>
       </c>
       <c r="D7">
-        <v>0.56359999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+        <v>0.77569999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
       <c r="B8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>0.59375</v>
+      </c>
+      <c r="D8">
+        <v>0.88480000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
       <c r="B9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>0.65625</v>
+      </c>
+      <c r="D9">
+        <v>0.76968999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10">
+        <v>0.71850000000000003</v>
+      </c>
+      <c r="D10">
         <v>0.72719999999999996</v>
       </c>
-      <c r="D10">
-        <v>0.71850000000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="2:4">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -2538,7 +3078,7 @@
         <v>0.58181000000000005</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4">
       <c r="B12" t="s">
         <v>20</v>
       </c>
@@ -2549,7 +3089,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4">
       <c r="B13" t="s">
         <v>21</v>
       </c>
@@ -2560,7 +3100,7 @@
         <v>0.46875</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4">
       <c r="B14" t="s">
         <v>22</v>
       </c>
@@ -2571,7 +3111,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4">
       <c r="B15" t="s">
         <v>29</v>
       </c>
@@ -2582,7 +3122,7 @@
         <v>0.29696899999999998</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -2593,7 +3133,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
         <v>24</v>
       </c>
@@ -2608,5 +3148,10 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>